<commit_message>
Finalizado el análisis estadístico de TP4.
</commit_message>
<xml_diff>
--- a/practica8/trunk/TP4/GrafoRegularAleatorio/AnálisisColoreo.xlsx
+++ b/practica8/trunk/TP4/GrafoRegularAleatorio/AnálisisColoreo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="798" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="798" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="50-regular 100-nodos" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <definedName name="_C005_grafo_250_regular_500_nodos" localSheetId="5">'250-regular 500-nodos'!$A$2:$B$11</definedName>
     <definedName name="_C006_grafo_350_regular_500_nodos" localSheetId="6">'350-regular 500-nodos'!$A$2:$B$15</definedName>
     <definedName name="_C007_grafo_500_regular_1000_nodos" localSheetId="7">'500-regular 1000-nodos'!$A$2:$B$13</definedName>
+    <definedName name="_C008_grafo_460_regular_5000_nodos" localSheetId="8">'460-regular 5000-nodos'!$A$2:$B$7</definedName>
     <definedName name="C000_grafo_50_regular_100_nodos" localSheetId="0">'50-regular 100-nodos'!$A$2:$B$9</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -91,6 +92,14 @@
   </connection>
   <connection id="8" name="C007-grafo-500-regular-1000-nodos" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="I:\dev\repos\progra3\practica8\trunk\TP4\GrafoRegularAleatorio\lote\salidas\secuencial\C007-grafo-500-regular-1000-nodos.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="C008-grafo-460-regular-5000-nodos" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="I:\dev\repos\progra3\practica8\trunk\TP4\GrafoRegularAleatorio\lote\salidas\secuencial\C008-grafo-460-regular-5000-nodos.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -199,7 +208,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -464,11 +472,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="123988992"/>
-        <c:axId val="106672512"/>
+        <c:axId val="104631680"/>
+        <c:axId val="105358464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="123988992"/>
+        <c:axId val="104631680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,7 +486,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106672512"/>
+        <c:crossAx val="105358464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -486,7 +494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106672512"/>
+        <c:axId val="105358464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,14 +517,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123988992"/>
+        <c:crossAx val="104631680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -575,7 +582,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -876,11 +882,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148281216"/>
-        <c:axId val="156950528"/>
+        <c:axId val="106841216"/>
+        <c:axId val="106842752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148281216"/>
+        <c:axId val="106841216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +896,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156950528"/>
+        <c:crossAx val="106842752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -898,7 +904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156950528"/>
+        <c:axId val="106842752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,14 +927,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148281216"/>
+        <c:crossAx val="106841216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -986,7 +991,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1305,11 +1309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132630400"/>
-        <c:axId val="132631936"/>
+        <c:axId val="106977920"/>
+        <c:axId val="106983808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132630400"/>
+        <c:axId val="106977920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1323,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132631936"/>
+        <c:crossAx val="106983808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132631936"/>
+        <c:axId val="106983808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,14 +1354,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132630400"/>
+        <c:crossAx val="106977920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1415,7 +1418,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1680,11 +1682,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="159960064"/>
-        <c:axId val="160015104"/>
+        <c:axId val="107073920"/>
+        <c:axId val="107075456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159960064"/>
+        <c:axId val="107073920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,7 +1696,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160015104"/>
+        <c:crossAx val="107075456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1702,7 +1704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160015104"/>
+        <c:axId val="107075456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,14 +1727,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159960064"/>
+        <c:crossAx val="107073920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1790,7 +1791,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2109,11 +2109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="160895360"/>
-        <c:axId val="160896896"/>
+        <c:axId val="107562496"/>
+        <c:axId val="107564032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="160895360"/>
+        <c:axId val="107562496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2123,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160896896"/>
+        <c:crossAx val="107564032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160896896"/>
+        <c:axId val="107564032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,14 +2154,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160895360"/>
+        <c:crossAx val="107562496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,7 +2218,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2520,11 +2518,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164222848"/>
-        <c:axId val="164224384"/>
+        <c:axId val="107639936"/>
+        <c:axId val="107641472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164222848"/>
+        <c:axId val="107639936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2534,7 +2532,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164224384"/>
+        <c:crossAx val="107641472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2542,7 +2540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164224384"/>
+        <c:axId val="107641472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,14 +2563,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164222848"/>
+        <c:crossAx val="107639936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2630,7 +2627,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3003,11 +2999,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="166480896"/>
-        <c:axId val="168162048"/>
+        <c:axId val="107412096"/>
+        <c:axId val="107417984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166480896"/>
+        <c:axId val="107412096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3017,7 +3013,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168162048"/>
+        <c:crossAx val="107417984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3025,7 +3021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168162048"/>
+        <c:axId val="107417984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3048,14 +3044,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166480896"/>
+        <c:crossAx val="107412096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3450,11 +3445,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168796544"/>
-        <c:axId val="168798080"/>
+        <c:axId val="107495808"/>
+        <c:axId val="107497344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168796544"/>
+        <c:axId val="107495808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3464,7 +3459,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168798080"/>
+        <c:crossAx val="107497344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3472,7 +3467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168798080"/>
+        <c:axId val="107497344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3502,7 +3497,346 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168796544"/>
+        <c:crossAx val="107495808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Distribución de Colores por Frecuencia</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'460-regular 5000-nodos'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'460-regular 5000-nodos'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matula</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'460-regular 5000-nodos'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Powell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'460-regular 5000-nodos'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="75116544"/>
+        <c:axId val="75118080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75116544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75118080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75118080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75116544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3805,6 +4139,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="C000-grafo-50-regular-100-nodos" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -3835,6 +4204,10 @@
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="C007-grafo-500-regular-1000-nodos" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="C008-grafo-460-regular-5000-nodos" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5777,7 +6150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D13"/>
     </sheetView>
   </sheetViews>
@@ -5995,16 +6368,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6022,7 +6395,109 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>96</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>225</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>98</v>
+      </c>
+      <c r="B4">
+        <v>3609</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>99</v>
+      </c>
+      <c r="B5">
+        <v>5137</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>998</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>101</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>10000</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:D8" si="0">SUM(C2:C7)</f>
+        <v>10000</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:D7">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>